<commit_message>
updated file to complete module 1
</commit_message>
<xml_diff>
--- a/final_project/qso320_final_project_raw_data_set.xlsx
+++ b/final_project/qso320_final_project_raw_data_set.xlsx
@@ -15,11 +15,14 @@
     <sheet name="qso320_final_project_raw_data_s" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId2"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="24">
   <si>
     <t>Sales</t>
   </si>
@@ -80,12 +83,25 @@
   <si>
     <t>Jan</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Sales</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -134,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,11 +168,39 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="9" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -167,6 +211,3361 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[qso320_final_project_raw_data_set.xlsx]qso320_final_project_raw_data_s!PivotTable3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Sales</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Red Wine - Last 6 Months</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0"/>
+              <a:t>By Sales Rep</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inBase"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>qso320_final_project_raw_data_s!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>qso320_final_project_raw_data_s!$J$5:$J$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Bill</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Jane</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Joe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>qso320_final_project_raw_data_s!$K$5:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0_);\("$"#,##0\)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>95536</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111937</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="463081344"/>
+        <c:axId val="463080952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="463081344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sales Representative</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463080952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="463080952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sales ($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463081344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[qso320_final_project_raw_data_set.xlsx]qso320_final_project_raw_data_s!PivotTable4</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Sales of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Wine - Last 6 Months</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0"/>
+              <a:t>by Wine Type</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inBase"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>qso320_final_project_raw_data_s!$H$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>qso320_final_project_raw_data_s!$G$30:$G$33</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Red</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>White</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>qso320_final_project_raw_data_s!$H$30:$H$33</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>166174</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>299361</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>301704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="461649000"/>
+        <c:axId val="461650960"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="461649000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Wine Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="461650960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="461650960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sales ($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="461649000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>736599</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Richard Lusch" refreshedDate="43108.811998379628" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="102">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E1048576" sheet="qso320_final_project_raw_data_s"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Sales" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3020" maxValue="11959"/>
+    </cacheField>
+    <cacheField name="City" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="Los Angeles"/>
+        <s v="San Francisco"/>
+        <s v="San Diego"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems containsBlank="1" count="7">
+        <s v="Feb"/>
+        <s v="Jun"/>
+        <s v="May"/>
+        <s v="Apr"/>
+        <s v="Mar"/>
+        <s v="Jan"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sales Rep" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="Bill"/>
+        <s v="Joe"/>
+        <s v="Jane"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Type Wine" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="Red"/>
+        <s v="Organic"/>
+        <s v="White"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="102">
+  <r>
+    <n v="7451"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="11221"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9525"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3986"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="11667"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11649"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9010"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5686"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9121"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8703"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4369"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5936"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9990"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5217"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5582"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7913"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8581"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7472"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4716"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="3020"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="11552"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8507"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8573"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4827"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="11146"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="10898"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="10424"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="6077"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4908"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4652"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7498"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4641"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="10440"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4168"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4031"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4031"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7498"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8305"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4788"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11953"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11482"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="11959"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8681"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="10399"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="11310"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6981"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8758"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9837"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4276"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7515"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="10497"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8587"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7373"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8722"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5607"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11029"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="6262"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9432"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6685"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3913"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7642"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9549"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9014"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7390"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3390"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4670"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8535"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9112"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8197"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3287"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6388"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9887"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6326"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="10694"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9779"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="10157"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5286"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8516"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7177"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="6312"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5546"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5294"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7879"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="6437"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6061"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7763"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5761"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9248"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="10919"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="11498"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8950"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9133"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9332"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5437"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7914"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8559"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8274"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="3877"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3407"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5605"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="G29:H33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="0" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="J4:K8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="5"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="4" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="0" baseField="3" baseItem="0" numFmtId="5"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G1:H5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="0" baseField="3" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="6">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,9 +3831,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -443,10 +3844,18 @@
     <col min="3" max="3" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="7.54296875" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" customWidth="1"/>
+    <col min="12" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.7265625" customWidth="1"/>
+    <col min="19" max="26" width="7.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +3871,20 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>7451</v>
       </c>
@@ -479,8 +3900,20 @@
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="9">
+        <v>245921</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>11221</v>
       </c>
@@ -496,8 +3929,14 @@
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9">
+        <v>269805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>9525</v>
       </c>
@@ -513,8 +3952,20 @@
       <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="9">
+        <v>251513</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3986</v>
       </c>
@@ -530,8 +3981,20 @@
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="9">
+        <v>767239</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="10">
+        <v>95536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>11667</v>
       </c>
@@ -547,8 +4010,14 @@
       <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="10">
+        <v>111937</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>11649</v>
       </c>
@@ -564,8 +4033,14 @@
       <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="10">
+        <v>91888</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>9010</v>
       </c>
@@ -581,8 +4056,14 @@
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="10">
+        <v>299361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>5686</v>
       </c>
@@ -599,7 +4080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9121</v>
       </c>
@@ -616,7 +4097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>8703</v>
       </c>
@@ -633,7 +4114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>4369</v>
       </c>
@@ -650,7 +4131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>5936</v>
       </c>
@@ -667,7 +4148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>9990</v>
       </c>
@@ -684,7 +4165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>5217</v>
       </c>
@@ -701,7 +4182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>5582</v>
       </c>
@@ -718,7 +4199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>7913</v>
       </c>
@@ -735,7 +4216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>8581</v>
       </c>
@@ -752,7 +4233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>7472</v>
       </c>
@@ -769,7 +4250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>4716</v>
       </c>
@@ -786,7 +4267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>3020</v>
       </c>
@@ -803,7 +4284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>11552</v>
       </c>
@@ -820,7 +4301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>8507</v>
       </c>
@@ -837,7 +4318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>8573</v>
       </c>
@@ -854,7 +4335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>4827</v>
       </c>
@@ -871,7 +4352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>11146</v>
       </c>
@@ -888,7 +4369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>10898</v>
       </c>
@@ -905,7 +4386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>10424</v>
       </c>
@@ -922,7 +4403,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>6077</v>
       </c>
@@ -938,8 +4419,14 @@
       <c r="E29" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>4908</v>
       </c>
@@ -955,8 +4442,14 @@
       <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="9">
+        <v>166174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>4652</v>
       </c>
@@ -972,8 +4465,14 @@
       <c r="E31" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="9">
+        <v>299361</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>7498</v>
       </c>
@@ -989,8 +4488,14 @@
       <c r="E32" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="9">
+        <v>301704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>4641</v>
       </c>
@@ -1006,8 +4511,14 @@
       <c r="E33" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="9">
+        <v>767239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>10440</v>
       </c>
@@ -1024,7 +4535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>4168</v>
       </c>
@@ -1041,7 +4552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>4031</v>
       </c>
@@ -1058,7 +4569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>4031</v>
       </c>
@@ -1075,7 +4586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>7498</v>
       </c>
@@ -1092,7 +4603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>8305</v>
       </c>
@@ -1109,7 +4620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>4788</v>
       </c>
@@ -1126,7 +4637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>11953</v>
       </c>
@@ -1143,7 +4654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>11482</v>
       </c>
@@ -1160,7 +4671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>11959</v>
       </c>
@@ -1177,7 +4688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>8681</v>
       </c>
@@ -1194,7 +4705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>10399</v>
       </c>
@@ -1211,7 +4722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>11310</v>
       </c>
@@ -1228,7 +4739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>6981</v>
       </c>
@@ -1245,7 +4756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>8758</v>
       </c>
@@ -2169,6 +5680,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>